<commit_message>
finish search engine at to_thai
</commit_message>
<xml_diff>
--- a/set_exching_rate.xlsx
+++ b/set_exching_rate.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="7">
   <si>
     <t>4010</t>
   </si>
@@ -53,7 +53,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,6 +85,12 @@
       <sz val="11.0"/>
       <i val="true"/>
       <color indexed="54"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+      <color indexed="20"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -125,7 +131,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -141,6 +147,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,28 +440,28 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="10">
+      <c r="A1" t="s" s="11">
         <v>6</v>
       </c>
-      <c r="B1" t="s" s="10">
+      <c r="B1" t="s" s="11">
         <v>0</v>
       </c>
       <c r="C1"/>
     </row>
     <row r="2">
-      <c r="A2" t="s" s="10">
+      <c r="A2" t="s" s="11">
         <v>2</v>
       </c>
-      <c r="B2" t="s" s="10">
+      <c r="B2" t="s" s="11">
         <v>3</v>
       </c>
       <c r="C2"/>
     </row>
     <row r="3">
-      <c r="A3" t="s" s="10">
+      <c r="A3" t="s" s="11">
         <v>4</v>
       </c>
-      <c r="B3" t="s" s="10">
+      <c r="B3" t="s" s="11">
         <v>5</v>
       </c>
       <c r="C3"/>

</xml_diff>

<commit_message>
add see more..... in to_thai
</commit_message>
<xml_diff>
--- a/set_exching_rate.xlsx
+++ b/set_exching_rate.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="8">
   <si>
     <t>4010</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>4000</t>
+  </si>
+  <si>
+    <t>4004</t>
   </si>
 </sst>
 </file>
@@ -53,7 +56,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,6 +88,12 @@
       <sz val="11.0"/>
       <i val="true"/>
       <color indexed="54"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+      <color indexed="20"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -131,7 +140,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -148,6 +157,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,28 +450,28 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="11">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s" s="11">
+      <c r="A1" t="s" s="12">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s" s="12">
         <v>0</v>
       </c>
       <c r="C1"/>
     </row>
     <row r="2">
-      <c r="A2" t="s" s="11">
+      <c r="A2" t="s" s="12">
         <v>2</v>
       </c>
-      <c r="B2" t="s" s="11">
+      <c r="B2" t="s" s="12">
         <v>3</v>
       </c>
       <c r="C2"/>
     </row>
     <row r="3">
-      <c r="A3" t="s" s="11">
+      <c r="A3" t="s" s="12">
         <v>4</v>
       </c>
-      <c r="B3" t="s" s="11">
+      <c r="B3" t="s" s="12">
         <v>5</v>
       </c>
       <c r="C3"/>

</xml_diff>

<commit_message>
completed separate inv_man m with ind_man m
</commit_message>
<xml_diff>
--- a/set_exching_rate.xlsx
+++ b/set_exching_rate.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="8">
   <si>
     <t>4010</t>
   </si>
@@ -56,7 +56,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,6 +88,18 @@
       <sz val="11.0"/>
       <i val="true"/>
       <color indexed="54"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+      <color indexed="20"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+      <color indexed="20"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -140,7 +152,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -158,6 +170,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,28 +464,28 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="12">
-        <v>7</v>
+      <c r="A1" t="s" s="14">
+        <v>6</v>
       </c>
-      <c r="B1" t="s" s="12">
+      <c r="B1" t="s" s="14">
         <v>0</v>
       </c>
       <c r="C1"/>
     </row>
     <row r="2">
-      <c r="A2" t="s" s="12">
+      <c r="A2" t="s" s="14">
         <v>2</v>
       </c>
-      <c r="B2" t="s" s="12">
+      <c r="B2" t="s" s="14">
         <v>3</v>
       </c>
       <c r="C2"/>
     </row>
     <row r="3">
-      <c r="A3" t="s" s="12">
+      <c r="A3" t="s" s="14">
         <v>4</v>
       </c>
-      <c r="B3" t="s" s="12">
+      <c r="B3" t="s" s="14">
         <v>5</v>
       </c>
       <c r="C3"/>

</xml_diff>